<commit_message>
Adjust input files and add additional files for PoC v02
</commit_message>
<xml_diff>
--- a/data/database/Data_Packages.xlsx
+++ b/data/database/Data_Packages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA65FCD-328D-40A7-8868-A85529FD7DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCFF2F8-31B5-4D87-9A65-473709D45F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataPackages" sheetId="111" r:id="rId1"/>
@@ -172,9 +172,6 @@
     <t>Format:</t>
   </si>
   <si>
-    <t>v0.0.1</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
   </si>
   <si>
     <t>Very first package, created for testing reasons</t>
+  </si>
+  <si>
+    <t>v0.0.2</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,12 @@
   </sheetPr>
   <dimension ref="B1:F11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -788,7 +793,7 @@
   <sheetData>
     <row r="1" spans="2:6" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
@@ -796,7 +801,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
@@ -807,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="2:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -815,10 +820,10 @@
         <v>2</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -826,10 +831,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:6" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -848,7 +853,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>3</v>
@@ -857,10 +862,10 @@
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="18"/>
       <c r="C8" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>17</v>
-      </c>
-      <c r="D8" s="16" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -883,12 +888,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1034,6 +1033,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1044,22 +1049,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1077,6 +1066,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Adjust database input files to new standards
Add descriptions everywhere
Have [MWh] everywhere (instead of sometimes [Mcal])
Have [p.u.] only when it is voltage or power, otherwise have [%, 0-1]
Rename SlopeVarCost to Efficiency
Rename InterVarCost to CommitConsumption
Rename StartupCost to StartupConsumption
</commit_message>
<xml_diff>
--- a/data/database/Data_Packages.xlsx
+++ b/data/database/Data_Packages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCFF2F8-31B5-4D87-9A65-473709D45F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97081849-7AE4-440E-B9A0-823025D3D3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-5835" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -787,7 +787,7 @@
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
     <col min="2" max="3" width="20" style="2" customWidth="1"/>
-    <col min="4" max="4" width="43.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="123" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -888,6 +888,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1033,22 +1048,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1064,28 +1088,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>